<commit_message>
ready to add trace
</commit_message>
<xml_diff>
--- a/王瀚庆-日志-20171016.xlsx
+++ b/王瀚庆-日志-20171016.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanghanqing/Documents/研究生/ForGraduation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\研究生\ForGraduation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12160" yWindow="800" windowWidth="32520" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="12165" yWindow="795" windowWidth="32520" windowHeight="20535" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="数据库设计" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>日期</t>
     <rPh sb="0" eb="1">
@@ -725,23 +723,89 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2017年10月16</t>
-    <rPh sb="4" eb="5">
-      <t>nian</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>yue</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开题报告初稿</t>
+    <t>1、完成开题报告</t>
     <rPh sb="0" eb="1">
       <t>kai'ti'bao'gao</t>
     </rPh>
     <rPh sb="4" eb="5">
       <t>chu'gao</t>
     </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、手机实验平台数据库设计，见sheet2，数据库设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据表1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>real</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据表2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPS201XXXXXlocationYY（时间地点次数）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PDR201XXXXXlocationYY（时间地点试验编号）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据表3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -807,7 +871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -827,11 +891,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="31" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="31" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -843,6 +906,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="31" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1123,17 +1194,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A7" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.6640625" customWidth="1"/>
+    <col min="4" max="4" width="77.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
@@ -1150,7 +1221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="180" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="171" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>42979</v>
       </c>
@@ -1164,7 +1235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>42980</v>
       </c>
@@ -1178,7 +1249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>42989</v>
       </c>
@@ -1192,7 +1263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>42995</v>
       </c>
@@ -1207,50 +1278,63 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>43017</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="225" x14ac:dyDescent="0.15">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
+    <row r="7" spans="1:4" ht="213.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="8">
+      <c r="A8" s="12">
         <v>43018</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+      <c r="A9" s="7">
+        <v>43029</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>22</v>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>43061</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1263,4 +1347,128 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B7:D7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>